<commit_message>
RDM-2055 Update spreadsheet with EndButtonLabel.
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V32_RDM-2055.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V32_RDM-2055.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-14060" yWindow="-28340" windowWidth="51200" windowHeight="28340" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="281">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -890,6 +890,18 @@
   </si>
   <si>
     <t>ShowEventNotes</t>
+  </si>
+  <si>
+    <t>Text value to show while submitting the event form data</t>
+  </si>
+  <si>
+    <t>EndButtonLabel</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>Create Draft</t>
   </si>
 </sst>
 </file>
@@ -1392,7 +1404,7 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1575,6 +1587,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -15992,8 +16008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="N1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -16101,7 +16117,9 @@
       <c r="R2" s="127" t="s">
         <v>275</v>
       </c>
-      <c r="S2" s="5"/>
+      <c r="S2" s="130" t="s">
+        <v>277</v>
+      </c>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
     </row>
@@ -16160,7 +16178,9 @@
       <c r="R3" s="128" t="s">
         <v>276</v>
       </c>
-      <c r="S3" s="8"/>
+      <c r="S3" s="131" t="s">
+        <v>278</v>
+      </c>
       <c r="T3" s="8"/>
       <c r="U3" s="8"/>
     </row>
@@ -16203,7 +16223,9 @@
       <c r="R4" s="129" t="s">
         <v>172</v>
       </c>
-      <c r="S4" s="4"/>
+      <c r="S4" s="120" t="s">
+        <v>279</v>
+      </c>
       <c r="T4" s="4"/>
       <c r="U4" s="4"/>
     </row>
@@ -16248,7 +16270,9 @@
       <c r="R5" s="129" t="s">
         <v>176</v>
       </c>
-      <c r="S5" s="4"/>
+      <c r="S5" s="120" t="s">
+        <v>280</v>
+      </c>
       <c r="T5" s="4"/>
       <c r="U5" s="4"/>
     </row>

</xml_diff>